<commit_message>
Removed the empty instances
</commit_message>
<xml_diff>
--- a/mappings/package_es16/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_es16/transformation/conceptual_mappings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1110B15-C22A-468F-92C2-9D199663CD52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9DE300FD-842F-4C75-86FA-2D7CEB43C878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,11 +24,11 @@
     <sheet name="CL2 Controlled List for Organis" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="Z_5728F340_C13A_42AA_8B8C_236E97D9F1E3_.wvu.FilterData" localSheetId="1" hidden="1">Rules!$A$1:$M$385</definedName>
+    <definedName name="Z_74E0F706_3AFB_4561_B266_7D2A699DC555_.wvu.FilterData" localSheetId="1" hidden="1">Rules!$A$1:$M$385</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
-    <customWorkbookView name="Identifiers" guid="{5728F340-C13A-42AA-8B8C-236E97D9F1E3}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Identifiers" guid="{74E0F706-3AFB-4561-B266-7D2A699DC555}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <fileRecoveryPr repairLoad="1"/>
   <extLst>
@@ -652,7 +652,7 @@
     <t>epo:Notice / epo:Notice / epo:Identifier / xsd:string</t>
   </si>
   <si>
-    <t>epo:refersToPrevious / epo:hasID / epo:hasIdentifierValue ?value</t>
+    <t>?this epo:refersToPrevious / epo:hasID / epo:hasIdentifierValue ?value</t>
   </si>
   <si>
     <t>I made the changes as pointed both in the CM ad TM for this one (Alex)</t>
@@ -21858,9 +21858,9 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{5728F340-C13A-42AA-8B8C-236E97D9F1E3}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{74E0F706-3AFB-4561-B266-7D2A699DC555}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:M385" xr:uid="{F64C7CC5-EE58-40A4-B298-FEC128F9194A}">
+      <autoFilter ref="A1:M385" xr:uid="{B27D2929-D6BF-40C8-A0FF-1E14964BD7C2}">
         <filterColumn colId="1">
           <customFilters>
             <customFilter val="*identifier*"/>

</xml_diff>

<commit_message>
Package finalized for release
</commit_message>
<xml_diff>
--- a/mappings/package_es16/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_es16/transformation/conceptual_mappings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\valexande\work\repos\ted-rdf-mapping\mappings\package_es16\transformation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5DB7BB-03ED-4752-BEAA-3BAB050C99DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55DDF223-BF8D-47D9-A6B2-D0221F691F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -24,17 +24,17 @@
     <sheet name="CL2 Controlled List for Organis" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="Z_ADD39E94_1EAF_45E2_AD62_C5236156DC0F_.wvu.FilterData" localSheetId="1" hidden="1">Rules!$A$1:$K$375</definedName>
+    <definedName name="Z_83138021_6814_4B21_A948_6285520CC7F5_.wvu.FilterData" localSheetId="1" hidden="1">Rules!$A$1:$K$375</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Identifiers" guid="{ADD39E94-1EAF-45E2-AD62-C5236156DC0F}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Identifiers" guid="{83138021-6814-4B21-A948-6285520CC7F5}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2620" uniqueCount="1982">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2621" uniqueCount="1983">
   <si>
     <t>Field</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>Mapping Version</t>
-  </si>
-  <si>
-    <t>1.0.0</t>
   </si>
   <si>
     <r>
@@ -289,6 +286,12 @@
     <t>/*/cbc:ID[@schemeName='notice-id']</t>
   </si>
   <si>
+    <t>epo:Notice / epo:Indentifier / rdf:langString</t>
+  </si>
+  <si>
+    <t>?this epo:hasID / epo:hasIdentifierValue ?value</t>
+  </si>
+  <si>
     <t>BT-757-notice BT-757-notice</t>
   </si>
   <si>
@@ -1556,9 +1559,6 @@
   </si>
   <si>
     <t>epo-not:PlanningNotice / epo:Identifier / xsd:string</t>
-  </si>
-  <si>
-    <t>?this epo:hasID / epo:hasIdentifierValue ?value</t>
   </si>
   <si>
     <t>BT-1251-Lot ND-Lot.ND-LotTenderingProcess.ND-LotPreviousPlanning.BT-1251-Lot</t>
@@ -6082,6 +6082,9 @@
   </si>
   <si>
     <t>?this epo:isSubjectToLotSpecificTerm / epo:hasBuyerCategoryDescription ?value .</t>
+  </si>
+  <si>
+    <t>1.1.1</t>
   </si>
 </sst>
 </file>
@@ -7028,9 +7031,9 @@
   </sheetPr>
   <dimension ref="A1:Y992"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -7089,32 +7092,32 @@
         <v>10</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>1982</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:25">
       <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:25">
       <c r="A8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="C8" s="11" t="s">
         <v>17</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>18</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="13"/>
@@ -7146,70 +7149,70 @@
     </row>
     <row r="10" spans="1:25">
       <c r="A10" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="15">
         <v>16</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:25">
       <c r="A12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="C12" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:25">
       <c r="A13" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="18"/>
       <c r="C13" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:25">
       <c r="A14" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="21"/>
     </row>
     <row r="15" spans="1:25">
       <c r="A15" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:25">
       <c r="A16" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="C16" s="23" t="s">
         <v>30</v>
-      </c>
-      <c r="C16" s="23" t="s">
-        <v>31</v>
       </c>
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
@@ -7236,13 +7239,13 @@
     </row>
     <row r="17" spans="1:25">
       <c r="A17" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="24" t="s">
-        <v>33</v>
-      </c>
       <c r="C17" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
@@ -10206,9 +10209,9 @@
   </sheetPr>
   <dimension ref="A1:Y403"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H157" sqref="H157"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G156" sqref="G156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -10227,7 +10230,7 @@
     <col min="15" max="15" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" ht="12.75">
       <c r="A1" s="26"/>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -10235,7 +10238,7 @@
       <c r="E1" s="29"/>
       <c r="F1" s="30"/>
       <c r="G1" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H1" s="27"/>
       <c r="I1" s="27"/>
@@ -10256,39 +10259,39 @@
       <c r="X1" s="31"/>
       <c r="Y1" s="31"/>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" ht="51">
       <c r="A2" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="C2" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="D2" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="E2" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="F2" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="G2" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="H2" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="I2" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="I2" s="34" t="s">
+      <c r="J2" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="J2" s="34" t="s">
+      <c r="K2" s="35" t="s">
         <v>44</v>
-      </c>
-      <c r="K2" s="35" t="s">
-        <v>45</v>
       </c>
       <c r="L2" s="31"/>
       <c r="M2" s="31"/>
@@ -10307,15 +10310,15 @@
     </row>
     <row r="3" spans="1:25" ht="15.75" customHeight="1">
       <c r="A3" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="38"/>
       <c r="D3" s="20"/>
       <c r="E3" s="37" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" s="20"/>
       <c r="G3" s="39"/>
@@ -10323,7 +10326,7 @@
       <c r="I3" s="20"/>
       <c r="J3" s="20"/>
       <c r="K3" s="41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L3" s="42"/>
       <c r="M3" s="42"/>
@@ -10334,19 +10337,19 @@
     </row>
     <row r="4" spans="1:25" ht="15.75" customHeight="1">
       <c r="A4" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="C4" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="D4" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="E4" s="37" t="s">
         <v>51</v>
-      </c>
-      <c r="E4" s="37" t="s">
-        <v>52</v>
       </c>
       <c r="F4" s="20"/>
       <c r="G4" s="39"/>
@@ -10354,7 +10357,7 @@
       <c r="I4" s="20"/>
       <c r="J4" s="20"/>
       <c r="K4" s="41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L4" s="42"/>
       <c r="M4" s="42"/>
@@ -10365,19 +10368,19 @@
     </row>
     <row r="5" spans="1:25" ht="15.75" customHeight="1">
       <c r="A5" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="C5" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="D5" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="E5" s="37" t="s">
         <v>56</v>
-      </c>
-      <c r="E5" s="37" t="s">
-        <v>57</v>
       </c>
       <c r="F5" s="20"/>
       <c r="G5" s="39"/>
@@ -10385,7 +10388,7 @@
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
       <c r="K5" s="41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L5" s="42"/>
       <c r="M5" s="42"/>
@@ -10396,19 +10399,19 @@
     </row>
     <row r="6" spans="1:25" ht="15.75" customHeight="1">
       <c r="A6" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="C6" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="D6" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="E6" s="37" t="s">
         <v>61</v>
-      </c>
-      <c r="E6" s="37" t="s">
-        <v>62</v>
       </c>
       <c r="F6" s="20"/>
       <c r="G6" s="39"/>
@@ -10416,7 +10419,7 @@
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
       <c r="K6" s="41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L6" s="42"/>
       <c r="M6" s="42"/>
@@ -10427,28 +10430,30 @@
     </row>
     <row r="7" spans="1:25" ht="15.75" customHeight="1">
       <c r="A7" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="C7" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="D7" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="E7" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="37" t="s">
+      <c r="F7" s="20"/>
+      <c r="G7" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="40"/>
+      <c r="H7" s="40" t="s">
+        <v>68</v>
+      </c>
       <c r="I7" s="20"/>
       <c r="J7" s="20"/>
-      <c r="K7" s="41" t="s">
-        <v>47</v>
-      </c>
+      <c r="K7" s="41"/>
       <c r="L7" s="42"/>
       <c r="M7" s="42"/>
       <c r="N7" s="42"/>
@@ -10458,19 +10463,19 @@
     </row>
     <row r="8" spans="1:25" ht="15.75" customHeight="1">
       <c r="A8" s="36" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C8" s="38" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F8" s="20"/>
       <c r="G8" s="39"/>
@@ -10478,7 +10483,7 @@
       <c r="I8" s="20"/>
       <c r="J8" s="20"/>
       <c r="K8" s="41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L8" s="42"/>
       <c r="M8" s="42"/>
@@ -10489,19 +10494,19 @@
     </row>
     <row r="9" spans="1:25" ht="15.75" customHeight="1">
       <c r="A9" s="36" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F9" s="20"/>
       <c r="G9" s="39"/>
@@ -10509,7 +10514,7 @@
       <c r="I9" s="20"/>
       <c r="J9" s="20"/>
       <c r="K9" s="41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L9" s="42"/>
       <c r="M9" s="42"/>
@@ -10520,19 +10525,19 @@
     </row>
     <row r="10" spans="1:25" ht="15.75" customHeight="1">
       <c r="A10" s="36" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C10" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F10" s="20"/>
       <c r="G10" s="39"/>
@@ -10540,7 +10545,7 @@
       <c r="I10" s="20"/>
       <c r="J10" s="20"/>
       <c r="K10" s="41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L10" s="42"/>
       <c r="M10" s="42"/>
@@ -10551,19 +10556,19 @@
     </row>
     <row r="11" spans="1:25" ht="15.75" customHeight="1">
       <c r="A11" s="36" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E11" s="37" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F11" s="20"/>
       <c r="G11" s="39"/>
@@ -10571,7 +10576,7 @@
       <c r="I11" s="20"/>
       <c r="J11" s="20"/>
       <c r="K11" s="41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L11" s="42"/>
       <c r="M11" s="42"/>
@@ -10582,19 +10587,19 @@
     </row>
     <row r="12" spans="1:25" ht="15.75" customHeight="1">
       <c r="A12" s="36" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F12" s="20"/>
       <c r="G12" s="39"/>
@@ -10602,7 +10607,7 @@
       <c r="I12" s="20"/>
       <c r="J12" s="20"/>
       <c r="K12" s="41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L12" s="42"/>
       <c r="M12" s="42"/>
@@ -10613,19 +10618,19 @@
     </row>
     <row r="13" spans="1:25" ht="15.75" customHeight="1">
       <c r="A13" s="36" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F13" s="20"/>
       <c r="G13" s="39"/>
@@ -10633,7 +10638,7 @@
       <c r="I13" s="20"/>
       <c r="J13" s="20"/>
       <c r="K13" s="41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L13" s="42"/>
       <c r="M13" s="42"/>
@@ -10644,17 +10649,17 @@
     </row>
     <row r="14" spans="1:25" ht="15.75" customHeight="1">
       <c r="A14" s="36" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C14" s="38" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="37" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F14" s="20"/>
       <c r="G14" s="39"/>
@@ -10662,7 +10667,7 @@
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
       <c r="K14" s="41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L14" s="42"/>
       <c r="M14" s="42"/>
@@ -10673,17 +10678,17 @@
     </row>
     <row r="15" spans="1:25" ht="15.75" customHeight="1">
       <c r="A15" s="43" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C15" s="38" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="37" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F15" s="20"/>
       <c r="G15" s="39"/>
@@ -10691,7 +10696,7 @@
       <c r="I15" s="20"/>
       <c r="J15" s="20"/>
       <c r="K15" s="41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L15" s="42"/>
       <c r="M15" s="42"/>
@@ -10702,22 +10707,22 @@
     </row>
     <row r="16" spans="1:25" ht="15.75" customHeight="1">
       <c r="A16" s="36" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C16" s="38"/>
       <c r="D16" s="20"/>
       <c r="E16" s="37" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F16" s="20"/>
       <c r="G16" s="39"/>
       <c r="H16" s="40"/>
       <c r="I16" s="20"/>
       <c r="J16" s="20" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="K16" s="41"/>
       <c r="L16" s="42"/>
@@ -10729,17 +10734,17 @@
     </row>
     <row r="17" spans="1:25" ht="15.75" customHeight="1">
       <c r="A17" s="44" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="37" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F17" s="20"/>
       <c r="G17" s="39"/>
@@ -10747,7 +10752,7 @@
       <c r="I17" s="20"/>
       <c r="J17" s="20"/>
       <c r="K17" s="41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L17" s="42"/>
       <c r="M17" s="42"/>
@@ -10758,15 +10763,15 @@
     </row>
     <row r="18" spans="1:25" ht="15.75" customHeight="1">
       <c r="A18" s="36" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C18" s="38"/>
       <c r="D18" s="20"/>
       <c r="E18" s="37" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F18" s="20"/>
       <c r="G18" s="39"/>
@@ -10783,17 +10788,17 @@
     </row>
     <row r="19" spans="1:25" ht="15.75" customHeight="1">
       <c r="A19" s="36" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C19" s="45" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="46" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F19" s="20"/>
       <c r="G19" s="40"/>
@@ -10801,7 +10806,7 @@
       <c r="I19" s="20"/>
       <c r="J19" s="20"/>
       <c r="K19" s="41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L19" s="42"/>
       <c r="M19" s="42"/>
@@ -10812,17 +10817,17 @@
     </row>
     <row r="20" spans="1:25" ht="15.75" customHeight="1">
       <c r="A20" s="36" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C20" s="45" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="37" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F20" s="20"/>
       <c r="G20" s="40"/>
@@ -10830,7 +10835,7 @@
       <c r="I20" s="20"/>
       <c r="J20" s="20"/>
       <c r="K20" s="41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L20" s="42"/>
       <c r="M20" s="42"/>
@@ -10841,17 +10846,17 @@
     </row>
     <row r="21" spans="1:25" ht="15.75" customHeight="1">
       <c r="A21" s="43" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B21" s="37" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C21" s="45" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="47" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F21" s="20"/>
       <c r="G21" s="48"/>
@@ -10859,7 +10864,7 @@
       <c r="I21" s="20"/>
       <c r="J21" s="20"/>
       <c r="K21" s="41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L21" s="42"/>
       <c r="M21" s="42"/>
@@ -10870,26 +10875,26 @@
     </row>
     <row r="22" spans="1:25" ht="15.75" customHeight="1">
       <c r="A22" s="43" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B22" s="37" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C22" s="38"/>
       <c r="D22" s="20"/>
       <c r="E22" s="37" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F22" s="20"/>
       <c r="G22" s="49" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H22" s="49" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I22" s="20"/>
       <c r="J22" s="20" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="K22" s="41"/>
       <c r="L22" s="42"/>
@@ -10901,26 +10906,26 @@
     </row>
     <row r="23" spans="1:25" ht="15.75" customHeight="1">
       <c r="A23" s="36" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B23" s="37" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C23" s="38"/>
       <c r="D23" s="20"/>
       <c r="E23" s="37" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F23" s="20"/>
       <c r="G23" s="40" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H23" s="40" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I23" s="20"/>
       <c r="J23" s="20" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="K23" s="41"/>
       <c r="L23" s="42"/>
@@ -10940,26 +10945,26 @@
     </row>
     <row r="24" spans="1:25" ht="15.75" customHeight="1">
       <c r="A24" s="36" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B24" s="37" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C24" s="38"/>
       <c r="D24" s="20"/>
       <c r="E24" s="37" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F24" s="20"/>
       <c r="G24" s="40" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H24" s="40" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I24" s="20"/>
       <c r="J24" s="20" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="K24" s="41"/>
       <c r="L24" s="42"/>
@@ -10979,31 +10984,31 @@
     </row>
     <row r="25" spans="1:25" ht="15.75" customHeight="1">
       <c r="A25" s="36" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B25" s="37" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C25" s="38" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="37" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F25" s="20"/>
       <c r="G25" s="49" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H25" s="49" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="I25" s="20"/>
       <c r="J25" s="20" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K25" s="41" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="L25" s="42"/>
       <c r="M25" s="42"/>
@@ -11014,30 +11019,30 @@
     </row>
     <row r="26" spans="1:25" ht="15.75" customHeight="1">
       <c r="A26" s="36" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B26" s="37" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C26" s="45" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E26" s="37" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F26" s="20"/>
       <c r="G26" s="49" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H26" s="49" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="I26" s="20"/>
       <c r="J26" s="20" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="K26" s="41"/>
       <c r="L26" s="42"/>
@@ -11049,30 +11054,30 @@
     </row>
     <row r="27" spans="1:25" ht="15.75" customHeight="1">
       <c r="A27" s="43" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B27" s="37" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C27" s="38" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E27" s="37" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F27" s="20"/>
       <c r="G27" s="49" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H27" s="49" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="I27" s="20"/>
       <c r="J27" s="20" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="K27" s="41"/>
       <c r="L27" s="42"/>
@@ -11084,30 +11089,30 @@
     </row>
     <row r="28" spans="1:25" ht="15.75" customHeight="1">
       <c r="A28" s="43" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B28" s="37" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C28" s="38" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E28" s="37" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F28" s="20"/>
       <c r="G28" s="49" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H28" s="49" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="I28" s="20"/>
       <c r="J28" s="20" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="K28" s="41"/>
       <c r="L28" s="42"/>
@@ -11119,22 +11124,22 @@
     </row>
     <row r="29" spans="1:25" ht="15.75" customHeight="1">
       <c r="A29" s="36" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B29" s="37" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C29" s="45"/>
       <c r="D29" s="20"/>
       <c r="E29" s="53" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F29" s="20"/>
       <c r="G29" s="40" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H29" s="40" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I29" s="20"/>
       <c r="J29" s="20"/>
@@ -11156,22 +11161,22 @@
     </row>
     <row r="30" spans="1:25" ht="15.75" customHeight="1">
       <c r="A30" s="36" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B30" s="37" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C30" s="45"/>
       <c r="D30" s="20"/>
       <c r="E30" s="47" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F30" s="20"/>
       <c r="G30" s="40" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H30" s="40" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="I30" s="20"/>
       <c r="J30" s="20"/>
@@ -11185,15 +11190,15 @@
     </row>
     <row r="31" spans="1:25" ht="15.75" customHeight="1">
       <c r="A31" s="43" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B31" s="37" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C31" s="45"/>
       <c r="D31" s="20"/>
       <c r="E31" s="46" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F31" s="20"/>
       <c r="G31" s="40"/>
@@ -11210,29 +11215,29 @@
     </row>
     <row r="32" spans="1:25" ht="15.75" customHeight="1">
       <c r="A32" s="36" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B32" s="37" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C32" s="38" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D32" s="20"/>
       <c r="E32" s="37" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F32" s="20"/>
       <c r="G32" s="40" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H32" s="40" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="I32" s="20"/>
       <c r="J32" s="20"/>
       <c r="K32" s="41" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="L32" s="42"/>
       <c r="M32" s="42"/>
@@ -11243,17 +11248,17 @@
     </row>
     <row r="33" spans="1:25" ht="15.75" customHeight="1">
       <c r="A33" s="36" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B33" s="37" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C33" s="45" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D33" s="20"/>
       <c r="E33" s="46" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F33" s="20"/>
       <c r="G33" s="40"/>
@@ -11261,7 +11266,7 @@
       <c r="I33" s="20"/>
       <c r="J33" s="20"/>
       <c r="K33" s="41" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="L33" s="42"/>
       <c r="M33" s="42"/>
@@ -11272,26 +11277,26 @@
     </row>
     <row r="34" spans="1:25" ht="15.75" customHeight="1">
       <c r="A34" s="43" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B34" s="37" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C34" s="38"/>
       <c r="D34" s="20"/>
       <c r="E34" s="37" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F34" s="20"/>
       <c r="G34" s="55" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H34" s="56" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="I34" s="20"/>
       <c r="J34" s="20" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K34" s="41"/>
       <c r="L34" s="42"/>
@@ -11303,27 +11308,27 @@
     </row>
     <row r="35" spans="1:25" ht="15.75" customHeight="1">
       <c r="A35" s="36" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B35" s="37" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C35" s="45" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D35" s="20"/>
       <c r="E35" s="37" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F35" s="20"/>
       <c r="G35" s="55"/>
       <c r="H35" s="56"/>
       <c r="I35" s="20"/>
       <c r="J35" s="20" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="K35" s="41" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="L35" s="50"/>
       <c r="M35" s="50"/>
@@ -11342,30 +11347,30 @@
     </row>
     <row r="36" spans="1:25" ht="15.75" customHeight="1">
       <c r="A36" s="36" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B36" s="37" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C36" s="38" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E36" s="37" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F36" s="20"/>
       <c r="G36" s="57" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H36" s="57" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="I36" s="20"/>
       <c r="J36" s="20" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="K36" s="41"/>
       <c r="L36" s="50"/>
@@ -11377,22 +11382,22 @@
     </row>
     <row r="37" spans="1:25" ht="15.75" customHeight="1">
       <c r="A37" s="43" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B37" s="37" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C37" s="38"/>
       <c r="D37" s="20"/>
       <c r="E37" s="37" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F37" s="20"/>
       <c r="G37" s="40" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H37" s="40" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="I37" s="20"/>
       <c r="J37" s="20"/>
@@ -11406,30 +11411,30 @@
     </row>
     <row r="38" spans="1:25" ht="15.75" customHeight="1">
       <c r="A38" s="36" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B38" s="37" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C38" s="45" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E38" s="37" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F38" s="20"/>
       <c r="G38" s="40" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="H38" s="40" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="I38" s="20"/>
       <c r="J38" s="20" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="K38" s="41"/>
       <c r="L38" s="50"/>
@@ -11441,30 +11446,30 @@
     </row>
     <row r="39" spans="1:25" ht="60">
       <c r="A39" s="36" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B39" s="37" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C39" s="38" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D39" s="20" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E39" s="37" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F39" s="20"/>
       <c r="G39" s="57" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H39" s="57" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="I39" s="20"/>
       <c r="J39" s="20" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="K39" s="41"/>
       <c r="L39" s="50"/>
@@ -11476,22 +11481,22 @@
     </row>
     <row r="40" spans="1:25" ht="45">
       <c r="A40" s="43" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B40" s="37" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C40" s="38"/>
       <c r="D40" s="20"/>
       <c r="E40" s="37" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F40" s="20"/>
       <c r="G40" s="40" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H40" s="40" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="I40" s="20"/>
       <c r="J40" s="20"/>
@@ -11513,30 +11518,30 @@
     </row>
     <row r="41" spans="1:25" ht="63">
       <c r="A41" s="36" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B41" s="37" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C41" s="45" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E41" s="46" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F41" s="20"/>
       <c r="G41" s="40" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="H41" s="40" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="I41" s="20"/>
       <c r="J41" s="20" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="K41" s="41"/>
       <c r="L41" s="42"/>
@@ -11548,30 +11553,30 @@
     </row>
     <row r="42" spans="1:25" ht="60">
       <c r="A42" s="36" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B42" s="37" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C42" s="38" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E42" s="37" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="F42" s="20"/>
       <c r="G42" s="57" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H42" s="57" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="I42" s="20"/>
       <c r="J42" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K42" s="41"/>
       <c r="L42" s="42"/>
@@ -11583,25 +11588,25 @@
     </row>
     <row r="43" spans="1:25" ht="45">
       <c r="A43" s="36" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B43" s="37" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C43" s="38"/>
       <c r="D43" s="20"/>
       <c r="E43" s="37" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F43" s="20"/>
       <c r="G43" s="40"/>
       <c r="H43" s="40"/>
       <c r="I43" s="20"/>
       <c r="J43" s="20" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="K43" s="41" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="L43" s="42"/>
       <c r="M43" s="42"/>
@@ -11612,30 +11617,30 @@
     </row>
     <row r="44" spans="1:25" ht="26.25">
       <c r="A44" s="36" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B44" s="37" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C44" s="38" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E44" s="37" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="F44" s="20"/>
       <c r="G44" s="40" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="H44" s="40" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="I44" s="20"/>
       <c r="J44" s="20" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="K44" s="41"/>
       <c r="L44" s="42"/>
@@ -11647,30 +11652,30 @@
     </row>
     <row r="45" spans="1:25">
       <c r="A45" s="36" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B45" s="37" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C45" s="38" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D45" s="20" t="s">
         <v>6</v>
       </c>
       <c r="E45" s="37" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F45" s="20"/>
       <c r="G45" s="48" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H45" s="22" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="I45" s="20"/>
       <c r="J45" s="20" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="K45" s="41"/>
       <c r="L45" s="42"/>
@@ -11682,30 +11687,30 @@
     </row>
     <row r="46" spans="1:25" ht="30">
       <c r="A46" s="43" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B46" s="37" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C46" s="38" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D46" s="20" t="s">
         <v>8</v>
       </c>
       <c r="E46" s="37" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F46" s="20"/>
       <c r="G46" s="58" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H46" s="58" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="I46" s="20"/>
       <c r="J46" s="20" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="K46" s="41"/>
       <c r="L46" s="42"/>
@@ -11717,30 +11722,30 @@
     </row>
     <row r="47" spans="1:25" ht="31.5">
       <c r="A47" s="36" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B47" s="37" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C47" s="45" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D47" s="20" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E47" s="46" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F47" s="20"/>
       <c r="G47" s="40" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="H47" s="40" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="I47" s="20"/>
       <c r="J47" s="20" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="K47" s="41"/>
       <c r="L47" s="42"/>
@@ -11752,30 +11757,30 @@
     </row>
     <row r="48" spans="1:25" ht="60">
       <c r="A48" s="43" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B48" s="37" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C48" s="38" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D48" s="20" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E48" s="37" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F48" s="20"/>
       <c r="G48" s="40" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="H48" s="40" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="I48" s="20"/>
       <c r="J48" s="20" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="K48" s="41"/>
       <c r="L48" s="42"/>
@@ -11787,15 +11792,15 @@
     </row>
     <row r="49" spans="1:25" ht="30">
       <c r="A49" s="36" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B49" s="37" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C49" s="38"/>
       <c r="D49" s="20"/>
       <c r="E49" s="37" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F49" s="20"/>
       <c r="G49" s="40"/>
@@ -11820,30 +11825,30 @@
     </row>
     <row r="50" spans="1:25" ht="45">
       <c r="A50" s="43" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B50" s="37" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C50" s="45" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E50" s="37" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F50" s="20"/>
       <c r="G50" s="40" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="H50" s="40" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="I50" s="20"/>
       <c r="J50" s="20" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="K50" s="41"/>
       <c r="L50" s="42"/>
@@ -11855,15 +11860,15 @@
     </row>
     <row r="51" spans="1:25" ht="60">
       <c r="A51" s="43" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B51" s="37" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C51" s="38"/>
       <c r="D51" s="20"/>
       <c r="E51" s="37" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F51" s="20"/>
       <c r="G51" s="39"/>
@@ -11880,30 +11885,30 @@
     </row>
     <row r="52" spans="1:25" ht="77.25">
       <c r="A52" s="36" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B52" s="37" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C52" s="38" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D52" s="20" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E52" s="37" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="F52" s="20"/>
       <c r="G52" s="39" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="H52" s="40" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="I52" s="20"/>
       <c r="J52" s="20" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="K52" s="41"/>
       <c r="L52" s="42"/>
@@ -11915,15 +11920,15 @@
     </row>
     <row r="53" spans="1:25" ht="45">
       <c r="A53" s="36" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B53" s="37" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C53" s="45"/>
       <c r="D53" s="20"/>
       <c r="E53" s="37" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="F53" s="20"/>
       <c r="G53" s="48"/>
@@ -11931,7 +11936,7 @@
       <c r="I53" s="20"/>
       <c r="J53" s="20"/>
       <c r="K53" s="41" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="L53" s="42"/>
       <c r="M53" s="42"/>
@@ -11942,15 +11947,15 @@
     </row>
     <row r="54" spans="1:25" ht="45">
       <c r="A54" s="43" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B54" s="37" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C54" s="38"/>
       <c r="D54" s="20"/>
       <c r="E54" s="37" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="F54" s="20"/>
       <c r="G54" s="40"/>
@@ -11967,19 +11972,19 @@
     </row>
     <row r="55" spans="1:25" ht="45">
       <c r="A55" s="36" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B55" s="37" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C55" s="38" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D55" s="20" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E55" s="37" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="F55" s="20"/>
       <c r="G55" s="40"/>
@@ -11996,19 +12001,19 @@
     </row>
     <row r="56" spans="1:25" ht="45">
       <c r="A56" s="36" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B56" s="37" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C56" s="45" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D56" s="20" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E56" s="37" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="F56" s="20"/>
       <c r="G56" s="40"/>
@@ -12025,15 +12030,15 @@
     </row>
     <row r="57" spans="1:25" ht="45">
       <c r="A57" s="43" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B57" s="37" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C57" s="38"/>
       <c r="D57" s="20"/>
       <c r="E57" s="37" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="F57" s="20"/>
       <c r="G57" s="40"/>
@@ -12041,7 +12046,7 @@
       <c r="I57" s="20"/>
       <c r="J57" s="20"/>
       <c r="K57" s="41" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="L57" s="42"/>
       <c r="M57" s="42"/>
@@ -12052,19 +12057,19 @@
     </row>
     <row r="58" spans="1:25" ht="45">
       <c r="A58" s="43" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B58" s="37" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C58" s="38" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D58" s="20" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E58" s="37" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="F58" s="20"/>
       <c r="G58" s="40"/>
@@ -12081,19 +12086,19 @@
     </row>
     <row r="59" spans="1:25" ht="45">
       <c r="A59" s="36" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B59" s="37" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C59" s="38" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D59" s="20" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E59" s="37" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="F59" s="20"/>
       <c r="G59" s="40"/>
@@ -12110,26 +12115,26 @@
     </row>
     <row r="60" spans="1:25" ht="60">
       <c r="A60" s="36" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B60" s="37" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C60" s="38"/>
       <c r="D60" s="20"/>
       <c r="E60" s="37" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F60" s="20"/>
       <c r="G60" s="40" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="H60" s="40" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="I60" s="20"/>
       <c r="J60" s="20" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="K60" s="41"/>
       <c r="L60" s="42"/>
@@ -12141,15 +12146,15 @@
     </row>
     <row r="61" spans="1:25" ht="45">
       <c r="A61" s="36" t="s">
+        <v>309</v>
+      </c>
+      <c r="B61" s="37" t="s">
         <v>308</v>
-      </c>
-      <c r="B61" s="37" t="s">
-        <v>307</v>
       </c>
       <c r="C61" s="38"/>
       <c r="D61" s="20"/>
       <c r="E61" s="37" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="F61" s="20"/>
       <c r="G61" s="40"/>
@@ -12166,30 +12171,30 @@
     </row>
     <row r="62" spans="1:25" ht="77.25">
       <c r="A62" s="36" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B62" s="37" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C62" s="38" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D62" s="20" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E62" s="37" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="F62" s="20"/>
       <c r="G62" s="40" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="H62" s="40" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="I62" s="20"/>
       <c r="J62" s="20" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="K62" s="41"/>
       <c r="L62" s="42"/>
@@ -12201,30 +12206,30 @@
     </row>
     <row r="63" spans="1:25" ht="77.25">
       <c r="A63" s="36" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B63" s="37" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C63" s="38" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D63" s="20" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E63" s="37" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="F63" s="20"/>
       <c r="G63" s="40" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="H63" s="40" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="I63" s="20"/>
       <c r="J63" s="20" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="K63" s="41"/>
       <c r="L63" s="42"/>
@@ -12236,30 +12241,30 @@
     </row>
     <row r="64" spans="1:25" ht="77.25">
       <c r="A64" s="36" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B64" s="37" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C64" s="38" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D64" s="20" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E64" s="37" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="F64" s="20"/>
       <c r="G64" s="40" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="H64" s="40" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="I64" s="20"/>
       <c r="J64" s="20" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="K64" s="41"/>
       <c r="L64" s="42"/>
@@ -12271,30 +12276,30 @@
     </row>
     <row r="65" spans="1:17" ht="77.25">
       <c r="A65" s="36" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B65" s="37" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C65" s="38" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D65" s="20" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E65" s="37" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F65" s="20"/>
       <c r="G65" s="40" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="H65" s="40" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="I65" s="20"/>
       <c r="J65" s="20" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="K65" s="41"/>
       <c r="L65" s="42"/>
@@ -12306,30 +12311,30 @@
     </row>
     <row r="66" spans="1:17" ht="77.25">
       <c r="A66" s="36" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B66" s="37" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C66" s="45" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D66" s="20" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E66" s="46" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="F66" s="20"/>
       <c r="G66" s="40" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="H66" s="40" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="I66" s="20"/>
       <c r="J66" s="20" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="K66" s="41"/>
       <c r="L66" s="42"/>
@@ -12341,30 +12346,30 @@
     </row>
     <row r="67" spans="1:17" ht="64.5">
       <c r="A67" s="36" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B67" s="37" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C67" s="45" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D67" s="20" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E67" s="37" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="F67" s="20"/>
       <c r="G67" s="40" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="H67" s="40" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="I67" s="20"/>
       <c r="J67" s="20" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="K67" s="41"/>
       <c r="L67" s="42"/>
@@ -12376,30 +12381,30 @@
     </row>
     <row r="68" spans="1:17" ht="77.25">
       <c r="A68" s="43" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B68" s="37" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C68" s="38" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D68" s="20" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E68" s="37" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="F68" s="20"/>
       <c r="G68" s="40" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="H68" s="40" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="I68" s="20"/>
       <c r="J68" s="20" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="K68" s="41"/>
       <c r="L68" s="42"/>
@@ -12411,30 +12416,30 @@
     </row>
     <row r="69" spans="1:17" ht="64.5">
       <c r="A69" s="43" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B69" s="37" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C69" s="38" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D69" s="20" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E69" s="37" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="F69" s="20"/>
       <c r="G69" s="40" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="H69" s="40" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="I69" s="20"/>
       <c r="J69" s="20" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="K69" s="41"/>
       <c r="L69" s="42"/>
@@ -12446,30 +12451,30 @@
     </row>
     <row r="70" spans="1:17" ht="64.5">
       <c r="A70" s="43" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B70" s="37" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C70" s="45" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D70" s="20" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="E70" s="46" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="F70" s="20"/>
       <c r="G70" s="59" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="H70" s="59" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="I70" s="20"/>
       <c r="J70" s="20" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="K70" s="41"/>
       <c r="L70" s="42"/>
@@ -12481,15 +12486,15 @@
     </row>
     <row r="71" spans="1:17">
       <c r="A71" s="36" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B71" s="37" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C71" s="38"/>
       <c r="D71" s="20"/>
       <c r="E71" s="37" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="F71" s="20"/>
       <c r="G71" s="40"/>
@@ -12506,15 +12511,15 @@
     </row>
     <row r="72" spans="1:17" ht="45">
       <c r="A72" s="36" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B72" s="37" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C72" s="38"/>
       <c r="D72" s="20"/>
       <c r="E72" s="37" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="F72" s="20"/>
       <c r="G72" s="40"/>
@@ -12531,26 +12536,26 @@
     </row>
     <row r="73" spans="1:17" ht="47.25">
       <c r="A73" s="43" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B73" s="37" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C73" s="45"/>
       <c r="D73" s="20"/>
       <c r="E73" s="46" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="F73" s="20"/>
       <c r="G73" s="40" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="H73" s="40" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="I73" s="20"/>
       <c r="J73" s="20" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="K73" s="41"/>
       <c r="L73" s="42"/>
@@ -12562,30 +12567,30 @@
     </row>
     <row r="74" spans="1:17" ht="60">
       <c r="A74" s="36" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B74" s="37" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C74" s="38" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D74" s="20" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="E74" s="37" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="F74" s="20"/>
       <c r="G74" s="40" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="H74" s="22" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="I74" s="20"/>
       <c r="J74" s="20" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="K74" s="41"/>
       <c r="L74" s="42"/>
@@ -12597,30 +12602,30 @@
     </row>
     <row r="75" spans="1:17" ht="45">
       <c r="A75" s="36" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B75" s="37" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C75" s="38" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D75" s="20" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="E75" s="37" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="F75" s="20"/>
       <c r="G75" s="22" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="H75" s="22" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="I75" s="20"/>
       <c r="J75" s="20" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="K75" s="41"/>
       <c r="L75" s="42"/>
@@ -12632,15 +12637,15 @@
     </row>
     <row r="76" spans="1:17" ht="47.25">
       <c r="A76" s="36" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B76" s="37" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C76" s="45"/>
       <c r="D76" s="20"/>
       <c r="E76" s="46" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="F76" s="20"/>
       <c r="G76" s="40"/>
@@ -12657,30 +12662,30 @@
     </row>
     <row r="77" spans="1:17" ht="63">
       <c r="A77" s="36" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B77" s="37" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C77" s="45" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D77" s="20" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="E77" s="46" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="F77" s="20"/>
       <c r="G77" s="40" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="H77" s="40" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="I77" s="20"/>
       <c r="J77" s="20" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="K77" s="41"/>
       <c r="L77" s="42"/>
@@ -12692,30 +12697,30 @@
     </row>
     <row r="78" spans="1:17" ht="60">
       <c r="A78" s="36" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B78" s="37" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C78" s="38" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D78" s="20" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="E78" s="37" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="F78" s="20"/>
       <c r="G78" s="40" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H78" s="40" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="I78" s="20"/>
       <c r="J78" s="20" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="K78" s="41"/>
       <c r="L78" s="42"/>
@@ -12727,30 +12732,30 @@
     </row>
     <row r="79" spans="1:17" ht="64.5">
       <c r="A79" s="36" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B79" s="60" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C79" s="61" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D79" s="62" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="E79" s="60" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="F79" s="20"/>
       <c r="G79" s="48" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="H79" s="48" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="I79" s="20"/>
       <c r="J79" s="20" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="K79" s="41"/>
       <c r="L79" s="42"/>
@@ -12762,30 +12767,30 @@
     </row>
     <row r="80" spans="1:17" ht="64.5">
       <c r="A80" s="36" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B80" s="37" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C80" s="38" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D80" s="20" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E80" s="37" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="F80" s="20"/>
       <c r="G80" s="40" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="H80" s="40" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="I80" s="20"/>
       <c r="J80" s="20" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="K80" s="41"/>
       <c r="L80" s="42"/>
@@ -12797,30 +12802,30 @@
     </row>
     <row r="81" spans="1:17" ht="60">
       <c r="A81" s="43" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B81" s="37" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C81" s="38" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D81" s="20" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E81" s="37" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="F81" s="20"/>
       <c r="G81" s="40" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="H81" s="40" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="I81" s="20"/>
       <c r="J81" s="20" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="K81" s="41"/>
       <c r="L81" s="42"/>
@@ -12832,30 +12837,30 @@
     </row>
     <row r="82" spans="1:17" ht="60">
       <c r="A82" s="36" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B82" s="37" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C82" s="38" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D82" s="20" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E82" s="37" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="F82" s="20"/>
       <c r="G82" s="40" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="H82" s="40" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="I82" s="20"/>
       <c r="J82" s="20" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="K82" s="41"/>
       <c r="L82" s="42"/>
@@ -12867,30 +12872,30 @@
     </row>
     <row r="83" spans="1:17">
       <c r="A83" s="36" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B83" s="37" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C83" s="38" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="D83" s="20" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="E83" s="37" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="F83" s="20"/>
       <c r="G83" s="40" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H83" s="40" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="I83" s="20"/>
       <c r="J83" s="20" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="K83" s="41"/>
       <c r="L83" s="42"/>
@@ -12902,30 +12907,30 @@
     </row>
     <row r="84" spans="1:17" ht="30">
       <c r="A84" s="36" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B84" s="37" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C84" s="38" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="D84" s="20" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="E84" s="37" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="F84" s="20"/>
       <c r="G84" s="40" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="H84" s="40" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="I84" s="20"/>
       <c r="J84" s="20" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="K84" s="41"/>
       <c r="L84" s="42"/>
@@ -12937,15 +12942,15 @@
     </row>
     <row r="85" spans="1:17" ht="47.25">
       <c r="A85" s="36" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B85" s="37" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C85" s="45"/>
       <c r="D85" s="20"/>
       <c r="E85" s="46" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="F85" s="20"/>
       <c r="G85" s="40"/>
@@ -12962,30 +12967,30 @@
     </row>
     <row r="86" spans="1:17" ht="75">
       <c r="A86" s="43" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B86" s="37" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C86" s="38" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="D86" s="20" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="E86" s="37" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="F86" s="20"/>
       <c r="G86" s="40" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="H86" s="48" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="I86" s="20"/>
       <c r="J86" s="20" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="K86" s="41"/>
       <c r="L86" s="42"/>
@@ -12997,30 +13002,30 @@
     </row>
     <row r="87" spans="1:17" ht="60">
       <c r="A87" s="36" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B87" s="37" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C87" s="45" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="D87" s="20" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="E87" s="37" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="F87" s="20"/>
       <c r="G87" s="48" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H87" s="40" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="I87" s="20"/>
       <c r="J87" s="20" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="K87" s="41"/>
       <c r="L87" s="42"/>
@@ -13032,33 +13037,33 @@
     </row>
     <row r="88" spans="1:17" ht="39">
       <c r="A88" s="43" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B88" s="37" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C88" s="45" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="D88" s="20" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="E88" s="46" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="F88" s="20"/>
       <c r="G88" s="40" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H88" s="40" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="I88" s="20"/>
       <c r="J88" s="20" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="K88" s="41" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="L88" s="42"/>
       <c r="M88" s="63"/>
@@ -13068,30 +13073,30 @@
     </row>
     <row r="89" spans="1:17" ht="26.25">
       <c r="A89" s="43" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B89" s="37" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C89" s="38" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="D89" s="20" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E89" s="37" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="F89" s="20"/>
       <c r="G89" s="40" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H89" s="40" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="I89" s="20"/>
       <c r="J89" s="20" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="K89" s="41"/>
       <c r="L89" s="42"/>
@@ -13102,26 +13107,26 @@
     </row>
     <row r="90" spans="1:17" ht="30">
       <c r="A90" s="36" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B90" s="37" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C90" s="45"/>
       <c r="D90" s="20"/>
       <c r="E90" s="37" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="F90" s="20"/>
       <c r="G90" s="40" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="H90" s="22" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="I90" s="20"/>
       <c r="J90" s="20" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="K90" s="41"/>
       <c r="L90" s="42"/>
@@ -13132,33 +13137,33 @@
     </row>
     <row r="91" spans="1:17" ht="30">
       <c r="A91" s="36" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B91" s="37" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C91" s="38" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="D91" s="20" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="E91" s="37" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="F91" s="20"/>
       <c r="G91" s="22" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="H91" s="22" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="I91" s="20"/>
       <c r="J91" s="20" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="K91" s="41" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="L91" s="42"/>
       <c r="M91" s="63"/>
@@ -13168,15 +13173,15 @@
     </row>
     <row r="92" spans="1:17" ht="30">
       <c r="A92" s="43" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B92" s="37" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C92" s="38"/>
       <c r="D92" s="20"/>
       <c r="E92" s="37" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="F92" s="20"/>
       <c r="G92" s="22"/>
@@ -13192,25 +13197,25 @@
     </row>
     <row r="93" spans="1:17" ht="47.25">
       <c r="A93" s="36" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B93" s="37" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="C93" s="45"/>
       <c r="D93" s="20"/>
       <c r="E93" s="46" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="F93" s="20"/>
       <c r="G93" s="40"/>
       <c r="H93" s="40"/>
       <c r="I93" s="20"/>
       <c r="J93" s="20" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="K93" s="41" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="L93" s="42"/>
       <c r="M93" s="63"/>
@@ -13220,30 +13225,30 @@
     </row>
     <row r="94" spans="1:17" ht="45">
       <c r="A94" s="36" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B94" s="37" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="C94" s="38" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="D94" s="20" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="E94" s="37" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="F94" s="20"/>
       <c r="G94" s="57" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="H94" s="57" t="s">
-        <v>490</v>
+        <v>68</v>
       </c>
       <c r="I94" s="20"/>
       <c r="J94" s="20" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="K94" s="41"/>
       <c r="L94" s="42"/>
@@ -13291,7 +13296,7 @@
         <v>498</v>
       </c>
       <c r="B96" s="37" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C96" s="38"/>
       <c r="D96" s="20"/>
@@ -13318,10 +13323,10 @@
         <v>501</v>
       </c>
       <c r="C97" s="38" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D97" s="20" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E97" s="37" t="s">
         <v>502</v>
@@ -13350,7 +13355,7 @@
         <v>505</v>
       </c>
       <c r="C98" s="38" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D98" s="20" t="s">
         <v>6</v>
@@ -13363,7 +13368,7 @@
         <v>507</v>
       </c>
       <c r="H98" s="22" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="I98" s="20"/>
       <c r="J98" s="20" t="s">
@@ -13384,7 +13389,7 @@
         <v>509</v>
       </c>
       <c r="C99" s="45" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D99" s="20" t="s">
         <v>8</v>
@@ -13397,7 +13402,7 @@
         <v>511</v>
       </c>
       <c r="H99" s="40" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="I99" s="20"/>
       <c r="J99" s="20" t="s">
@@ -13418,10 +13423,10 @@
         <v>513</v>
       </c>
       <c r="C100" s="38" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D100" s="20" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E100" s="37" t="s">
         <v>514</v>
@@ -13452,10 +13457,10 @@
         <v>518</v>
       </c>
       <c r="C101" s="38" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D101" s="20" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E101" s="37" t="s">
         <v>519</v>
@@ -13588,10 +13593,10 @@
         <v>543</v>
       </c>
       <c r="C105" s="38" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D105" s="20" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E105" s="37" t="s">
         <v>544</v>
@@ -13670,10 +13675,10 @@
         <v>554</v>
       </c>
       <c r="C108" s="38" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D108" s="20" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E108" s="37" t="s">
         <v>555</v>
@@ -13698,10 +13703,10 @@
         <v>557</v>
       </c>
       <c r="C109" s="38" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D109" s="20" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E109" s="37" t="s">
         <v>552</v>
@@ -13736,7 +13741,7 @@
       <c r="I110" s="20"/>
       <c r="J110" s="20"/>
       <c r="K110" s="41" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="L110" s="42"/>
       <c r="M110" s="63"/>
@@ -13752,10 +13757,10 @@
         <v>562</v>
       </c>
       <c r="C111" s="38" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D111" s="20" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E111" s="37" t="s">
         <v>563</v>
@@ -13780,10 +13785,10 @@
         <v>565</v>
       </c>
       <c r="C112" s="38" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D112" s="20" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E112" s="37" t="s">
         <v>566</v>
@@ -14084,10 +14089,10 @@
       </c>
       <c r="F122" s="20"/>
       <c r="G122" s="40" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="H122" s="40" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="I122" s="20"/>
       <c r="J122" s="20" t="s">
@@ -14132,10 +14137,10 @@
         <v>623</v>
       </c>
       <c r="C124" s="38" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D124" s="20" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E124" s="37" t="s">
         <v>624</v>
@@ -14145,7 +14150,7 @@
         <v>625</v>
       </c>
       <c r="H124" s="40" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="I124" s="20"/>
       <c r="J124" s="20" t="s">
@@ -14166,10 +14171,10 @@
         <v>627</v>
       </c>
       <c r="C125" s="38" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D125" s="20" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E125" s="37" t="s">
         <v>628</v>
@@ -14200,10 +14205,10 @@
         <v>631</v>
       </c>
       <c r="C126" s="38" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D126" s="20" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E126" s="37" t="s">
         <v>632</v>
@@ -14213,7 +14218,7 @@
         <v>625</v>
       </c>
       <c r="H126" s="40" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="I126" s="20"/>
       <c r="J126" s="20" t="s">
@@ -14234,10 +14239,10 @@
         <v>634</v>
       </c>
       <c r="C127" s="38" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D127" s="20" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E127" s="37" t="s">
         <v>635</v>
@@ -14247,7 +14252,7 @@
         <v>625</v>
       </c>
       <c r="H127" s="40" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="I127" s="20"/>
       <c r="J127" s="20" t="s">
@@ -14268,10 +14273,10 @@
         <v>637</v>
       </c>
       <c r="C128" s="38" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D128" s="20" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E128" s="37" t="s">
         <v>638</v>
@@ -14281,7 +14286,7 @@
         <v>625</v>
       </c>
       <c r="H128" s="40" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="I128" s="20"/>
       <c r="J128" s="20" t="s">
@@ -14302,10 +14307,10 @@
         <v>640</v>
       </c>
       <c r="C129" s="38" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D129" s="20" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E129" s="37" t="s">
         <v>641</v>
@@ -14315,7 +14320,7 @@
         <v>642</v>
       </c>
       <c r="H129" s="40" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="I129" s="20"/>
       <c r="J129" s="20" t="s">
@@ -14336,10 +14341,10 @@
         <v>644</v>
       </c>
       <c r="C130" s="45" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D130" s="20" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E130" s="46" t="s">
         <v>645</v>
@@ -14349,7 +14354,7 @@
         <v>646</v>
       </c>
       <c r="H130" s="40" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="I130" s="20"/>
       <c r="J130" s="20" t="s">
@@ -14370,10 +14375,10 @@
         <v>648</v>
       </c>
       <c r="C131" s="45" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D131" s="20" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E131" s="46" t="s">
         <v>649</v>
@@ -14383,7 +14388,7 @@
         <v>650</v>
       </c>
       <c r="H131" s="40" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="I131" s="20"/>
       <c r="J131" s="20" t="s">
@@ -14404,10 +14409,10 @@
         <v>652</v>
       </c>
       <c r="C132" s="38" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D132" s="20" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="E132" s="37" t="s">
         <v>653</v>
@@ -14696,10 +14701,10 @@
       </c>
       <c r="F141" s="20"/>
       <c r="G141" s="40" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="H141" s="40" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="I141" s="20"/>
       <c r="J141" s="20"/>
@@ -15272,10 +15277,10 @@
         <v>805</v>
       </c>
       <c r="C160" s="38" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D160" s="20" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E160" s="37" t="s">
         <v>806</v>
@@ -15632,10 +15637,10 @@
         <v>855</v>
       </c>
       <c r="C173" s="45" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="D173" s="20" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E173" s="46" t="s">
         <v>856</v>
@@ -15645,7 +15650,7 @@
         <v>511</v>
       </c>
       <c r="H173" s="40" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="I173" s="20"/>
       <c r="J173" s="20" t="s">
@@ -16315,7 +16320,7 @@
         <v>974</v>
       </c>
       <c r="B195" s="37" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C195" s="38"/>
       <c r="D195" s="38"/>
@@ -16331,7 +16336,7 @@
       </c>
       <c r="I195" s="20"/>
       <c r="J195" s="20" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="K195" s="41"/>
       <c r="L195" s="42"/>
@@ -17768,10 +17773,10 @@
         <v>1219</v>
       </c>
       <c r="C242" s="45" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D242" s="20" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E242" s="46" t="s">
         <v>1220</v>
@@ -17802,17 +17807,17 @@
         <v>1219</v>
       </c>
       <c r="C243" s="38" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D243" s="20" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E243" s="37" t="s">
         <v>1220</v>
       </c>
       <c r="F243" s="20"/>
       <c r="G243" s="40" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="H243" s="40" t="s">
         <v>1223</v>
@@ -19260,7 +19265,7 @@
       <c r="I290" s="20"/>
       <c r="J290" s="20"/>
       <c r="K290" s="41" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="L290" s="42"/>
       <c r="M290" s="63"/>
@@ -19287,7 +19292,7 @@
         <v>1460</v>
       </c>
       <c r="H291" s="40" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I291" s="20"/>
       <c r="J291" s="20"/>
@@ -19324,7 +19329,7 @@
       <c r="I292" s="20"/>
       <c r="J292" s="20"/>
       <c r="K292" s="41" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="L292" s="42"/>
       <c r="M292" s="63"/>
@@ -19351,7 +19356,7 @@
         <v>1467</v>
       </c>
       <c r="H293" s="40" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I293" s="20"/>
       <c r="J293" s="20"/>
@@ -19426,10 +19431,10 @@
         <v>1476</v>
       </c>
       <c r="C296" s="38" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="D296" s="20" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="E296" s="37" t="s">
         <v>1477</v>
@@ -19596,10 +19601,10 @@
         <v>1502</v>
       </c>
       <c r="C302" s="38" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D302" s="20" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E302" s="37" t="s">
         <v>1503</v>
@@ -19628,7 +19633,7 @@
         <v>1506</v>
       </c>
       <c r="C303" s="45" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D303" s="20" t="s">
         <v>6</v>
@@ -19660,7 +19665,7 @@
         <v>1510</v>
       </c>
       <c r="C304" s="38" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D304" s="20" t="s">
         <v>8</v>
@@ -19724,10 +19729,10 @@
         <v>1518</v>
       </c>
       <c r="C306" s="38" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D306" s="20" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E306" s="37" t="s">
         <v>1519</v>
@@ -19793,7 +19798,7 @@
         <v>1529</v>
       </c>
       <c r="H308" s="40" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="I308" s="20"/>
       <c r="J308" s="20" t="s">
@@ -19862,10 +19867,10 @@
         <v>1537</v>
       </c>
       <c r="C311" s="38" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D311" s="20" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E311" s="37" t="s">
         <v>1538</v>
@@ -19894,10 +19899,10 @@
         <v>1541</v>
       </c>
       <c r="C312" s="38" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="D312" s="20" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E312" s="37" t="s">
         <v>1542</v>
@@ -20845,7 +20850,7 @@
         <v>1691</v>
       </c>
       <c r="H343" s="40" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="I343" s="20"/>
       <c r="J343" s="20" t="s">
@@ -21419,12 +21424,12 @@
         <v>1794</v>
       </c>
       <c r="H360" s="40" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="I360" s="20"/>
       <c r="J360" s="20"/>
       <c r="K360" s="41" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="L360" s="42"/>
       <c r="M360" s="63"/>
@@ -21451,7 +21456,7 @@
         <v>1795</v>
       </c>
       <c r="H361" s="40" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I361" s="20"/>
       <c r="J361" s="20"/>
@@ -21483,12 +21488,12 @@
         <v>1800</v>
       </c>
       <c r="H362" s="40" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="I362" s="20"/>
       <c r="J362" s="20"/>
       <c r="K362" s="41" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="L362" s="42"/>
       <c r="M362" s="63"/>
@@ -21515,7 +21520,7 @@
         <v>1801</v>
       </c>
       <c r="H363" s="40" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I363" s="20"/>
       <c r="J363" s="20"/>
@@ -21547,12 +21552,12 @@
         <v>1805</v>
       </c>
       <c r="H364" s="40" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="I364" s="20"/>
       <c r="J364" s="20"/>
       <c r="K364" s="41" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="L364" s="42"/>
       <c r="M364" s="63"/>
@@ -21579,7 +21584,7 @@
         <v>1806</v>
       </c>
       <c r="H365" s="40" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I365" s="20"/>
       <c r="J365" s="20"/>
@@ -22390,9 +22395,9 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{ADD39E94-1EAF-45E2-AD62-C5236156DC0F}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{83138021-6814-4B21-A948-6285520CC7F5}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:K375" xr:uid="{20D00205-97CB-4943-A151-F970833B3EA9}">
+      <autoFilter ref="A1:K375" xr:uid="{46F4071B-9D5E-433F-8831-ACBD87C1EBB2}">
         <filterColumn colId="1">
           <customFilters>
             <customFilter val="*identifier*"/>
@@ -22469,19 +22474,19 @@
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" s="73" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="C1" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="D1" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="E1" s="28" t="s">
         <v>38</v>
-      </c>
-      <c r="E1" s="28" t="s">
-        <v>39</v>
       </c>
       <c r="F1" s="28" t="s">
         <v>2</v>
@@ -26932,7 +26937,7 @@
     <col min="5" max="5" width="32.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" ht="12.75">
       <c r="A1" s="100" t="s">
         <v>1934</v>
       </c>
@@ -26946,7 +26951,7 @@
       </c>
       <c r="F1" s="101"/>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" ht="12.75">
       <c r="A2" s="80" t="s">
         <v>1937</v>
       </c>
@@ -26963,7 +26968,7 @@
         <v>1941</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" ht="12.75">
       <c r="A3" s="75" t="s">
         <v>1942</v>
       </c>
@@ -27001,7 +27006,7 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" ht="12.75">
       <c r="A4" s="92" t="s">
         <v>1947</v>
       </c>
@@ -27039,7 +27044,7 @@
       <c r="Y4" s="23"/>
       <c r="Z4" s="23"/>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" ht="12.75">
       <c r="A5" s="75" t="s">
         <v>1949</v>
       </c>
@@ -27073,7 +27078,7 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" ht="12.75">
       <c r="A6" s="3" t="s">
         <v>1951</v>
       </c>
@@ -27111,7 +27116,7 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" ht="12.75">
       <c r="A7" s="3" t="s">
         <v>1954</v>
       </c>
@@ -27149,7 +27154,7 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" ht="12.75">
       <c r="A8" s="3" t="s">
         <v>1957</v>
       </c>
@@ -27187,7 +27192,7 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" ht="12.75">
       <c r="A9" s="95" t="s">
         <v>1960</v>
       </c>
@@ -27225,7 +27230,7 @@
       <c r="Y9" s="96"/>
       <c r="Z9" s="96"/>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:26" ht="12.75">
       <c r="A10" s="95" t="s">
         <v>1963</v>
       </c>
@@ -27263,7 +27268,7 @@
       <c r="Y10" s="96"/>
       <c r="Z10" s="96"/>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" ht="12.75">
       <c r="A11" s="95" t="s">
         <v>1965</v>
       </c>
@@ -27301,7 +27306,7 @@
       <c r="Y11" s="96"/>
       <c r="Z11" s="96"/>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" ht="12.75">
       <c r="A12" s="95" t="s">
         <v>1968</v>
       </c>
@@ -27339,7 +27344,7 @@
       <c r="Y12" s="96"/>
       <c r="Z12" s="96"/>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" ht="12.75">
       <c r="A13" s="95" t="s">
         <v>1970</v>
       </c>
@@ -27377,7 +27382,7 @@
       <c r="Y13" s="96"/>
       <c r="Z13" s="96"/>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" ht="12.75">
       <c r="A14" s="95" t="s">
         <v>1972</v>
       </c>
@@ -27415,7 +27420,7 @@
       <c r="Y14" s="96"/>
       <c r="Z14" s="96"/>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" ht="12.75">
       <c r="E15" s="13"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1">
@@ -27426,7 +27431,7 @@
         <v>1944</v>
       </c>
       <c r="E16" s="98" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="15.75" customHeight="1">
@@ -27437,61 +27442,61 @@
         <v>1944</v>
       </c>
       <c r="E17" s="98" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="12.75">
       <c r="E18" s="13"/>
     </row>
-    <row r="19" spans="2:5">
+    <row r="19" spans="2:5" ht="12.75">
       <c r="E19" s="13"/>
     </row>
-    <row r="20" spans="2:5">
+    <row r="20" spans="2:5" ht="12.75">
       <c r="E20" s="13"/>
     </row>
-    <row r="21" spans="2:5">
+    <row r="21" spans="2:5" ht="12.75">
       <c r="E21" s="13"/>
     </row>
-    <row r="22" spans="2:5">
+    <row r="22" spans="2:5" ht="12.75">
       <c r="E22" s="13"/>
     </row>
-    <row r="23" spans="2:5">
+    <row r="23" spans="2:5" ht="12.75">
       <c r="E23" s="13"/>
     </row>
-    <row r="24" spans="2:5">
+    <row r="24" spans="2:5" ht="12.75">
       <c r="E24" s="13"/>
     </row>
-    <row r="25" spans="2:5">
+    <row r="25" spans="2:5" ht="12.75">
       <c r="E25" s="13"/>
     </row>
-    <row r="26" spans="2:5">
+    <row r="26" spans="2:5" ht="12.75">
       <c r="E26" s="13"/>
     </row>
-    <row r="27" spans="2:5">
+    <row r="27" spans="2:5" ht="12.75">
       <c r="E27" s="13"/>
     </row>
-    <row r="28" spans="2:5">
+    <row r="28" spans="2:5" ht="12.75">
       <c r="E28" s="13"/>
     </row>
-    <row r="29" spans="2:5">
+    <row r="29" spans="2:5" ht="12.75">
       <c r="E29" s="13"/>
     </row>
-    <row r="30" spans="2:5">
+    <row r="30" spans="2:5" ht="12.75">
       <c r="E30" s="13"/>
     </row>
-    <row r="31" spans="2:5">
+    <row r="31" spans="2:5" ht="12.75">
       <c r="E31" s="13"/>
     </row>
-    <row r="32" spans="2:5">
+    <row r="32" spans="2:5" ht="12.75">
       <c r="E32" s="13"/>
     </row>
-    <row r="33" spans="5:5">
+    <row r="33" spans="5:5" ht="12.75">
       <c r="E33" s="13"/>
     </row>
-    <row r="34" spans="5:5">
+    <row r="34" spans="5:5" ht="12.75">
       <c r="E34" s="13"/>
     </row>
-    <row r="35" spans="5:5">
+    <row r="35" spans="5:5" ht="12.75">
       <c r="E35" s="13"/>
     </row>
     <row r="36" spans="5:5" ht="12.75">
@@ -30446,7 +30451,7 @@
         <v>1977</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -30457,7 +30462,7 @@
         <v>1979</v>
       </c>
       <c r="C5" s="99" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D5" s="25" t="s">
         <v>1980</v>

</xml_diff>